<commit_message>
Dam and fishway template updates
Changes to construction_type allowable values and all feature type attributes displayed by default.
</commit_message>
<xml_diff>
--- a/docs/source/docs_user/downloads/fishwaystemplate06222022.xlsx
+++ b/docs/source/docs_user/downloads/fishwaystemplate06222022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CABD\GitHub\Canadian-Wildlife-Federation\Documentation\docs\source\docs_user\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E7AF127-C956-4227-BEB0-4EA92B31F75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CD763A-2C27-4353-9854-A8FC61BAF529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29370" yWindow="570" windowWidth="18435" windowHeight="14640" activeTab="1" xr2:uid="{D1F32723-011C-4BB5-A383-35CF3049E8BB}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{D1F32723-011C-4BB5-A383-35CF3049E8BB}"/>
   </bookViews>
   <sheets>
     <sheet name="new_data" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>entry_classification</t>
   </si>
@@ -271,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -288,11 +288,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -302,6 +322,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,24 +641,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2B8F55-CB36-49BA-83DD-053178AEA116}">
-  <dimension ref="A1:Z50"/>
+  <dimension ref="A1:AO50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="26.08984375" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" customWidth="1"/>
-    <col min="5" max="5" width="11.6328125" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="7" max="26" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="26.36328125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="29.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -652,75 +712,120 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
+      <c r="G1" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="6"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -740,15 +845,30 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="6"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -768,15 +888,30 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -796,15 +931,30 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -824,15 +974,30 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -852,15 +1017,30 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -880,15 +1060,30 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -908,15 +1103,30 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -936,15 +1146,30 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -964,15 +1189,30 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -992,15 +1232,30 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1020,15 +1275,30 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1048,15 +1318,30 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1076,15 +1361,30 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1104,15 +1404,30 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1132,15 +1447,30 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="2"/>
+      <c r="AN16" s="2"/>
+      <c r="AO16" s="2"/>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1160,15 +1490,30 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="2"/>
+      <c r="AN17" s="2"/>
+      <c r="AO17" s="2"/>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1188,15 +1533,30 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="2"/>
+      <c r="AN18" s="2"/>
+      <c r="AO18" s="2"/>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1216,15 +1576,30 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="2"/>
+      <c r="AO19" s="2"/>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1244,15 +1619,30 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="2"/>
+      <c r="AN20" s="2"/>
+      <c r="AO20" s="2"/>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1272,15 +1662,30 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -1300,15 +1705,30 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -1328,15 +1748,30 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="G24" s="6"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1356,15 +1791,30 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="6"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1384,15 +1834,30 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1412,15 +1877,30 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1440,15 +1920,30 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="2"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="6"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1468,15 +1963,30 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="2"/>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="G29" s="6"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1496,15 +2006,30 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA29" s="2"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="2"/>
+      <c r="AE29" s="2"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="2"/>
+      <c r="AI29" s="2"/>
+      <c r="AJ29" s="2"/>
+      <c r="AK29" s="2"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="2"/>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="2"/>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="G30" s="6"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -1524,15 +2049,30 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="2"/>
+      <c r="AI30" s="2"/>
+      <c r="AJ30" s="2"/>
+      <c r="AK30" s="2"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="2"/>
+      <c r="AN30" s="2"/>
+      <c r="AO30" s="2"/>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="6"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -1552,15 +2092,30 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA31" s="2"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="2"/>
+      <c r="AE31" s="2"/>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="2"/>
+      <c r="AI31" s="2"/>
+      <c r="AJ31" s="2"/>
+      <c r="AK31" s="2"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="2"/>
+      <c r="AN31" s="2"/>
+      <c r="AO31" s="2"/>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="G32" s="6"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -1580,15 +2135,30 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="2"/>
+      <c r="AK32" s="2"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="2"/>
+      <c r="AN32" s="2"/>
+      <c r="AO32" s="2"/>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="G33" s="6"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1608,15 +2178,30 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="2"/>
+      <c r="AE33" s="2"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="2"/>
+      <c r="AK33" s="2"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+    </row>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="G34" s="6"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -1636,15 +2221,30 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
+      <c r="AJ34" s="2"/>
+      <c r="AK34" s="2"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
+    </row>
+    <row r="35" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="G35" s="6"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -1664,15 +2264,30 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="2"/>
+      <c r="AE35" s="2"/>
+      <c r="AF35" s="2"/>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2"/>
+      <c r="AI35" s="2"/>
+      <c r="AJ35" s="2"/>
+      <c r="AK35" s="2"/>
+      <c r="AL35" s="2"/>
+      <c r="AM35" s="2"/>
+      <c r="AN35" s="2"/>
+      <c r="AO35" s="2"/>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="G36" s="6"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -1692,15 +2307,30 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="2"/>
+      <c r="AE36" s="2"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="2"/>
+      <c r="AI36" s="2"/>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="2"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+    </row>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="G37" s="6"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -1720,15 +2350,30 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2"/>
+      <c r="AF37" s="2"/>
+      <c r="AG37" s="2"/>
+      <c r="AH37" s="2"/>
+      <c r="AI37" s="2"/>
+      <c r="AJ37" s="2"/>
+      <c r="AK37" s="2"/>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="2"/>
+      <c r="AN37" s="2"/>
+      <c r="AO37" s="2"/>
+    </row>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="6"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1748,15 +2393,30 @@
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="2"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="2"/>
+      <c r="AI38" s="2"/>
+      <c r="AJ38" s="2"/>
+      <c r="AK38" s="2"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="6"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -1776,15 +2436,30 @@
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="2"/>
+      <c r="AE39" s="2"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AI39" s="2"/>
+      <c r="AJ39" s="2"/>
+      <c r="AK39" s="2"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="G40" s="6"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -1804,15 +2479,30 @@
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="2"/>
+      <c r="AE40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AI40" s="2"/>
+      <c r="AJ40" s="2"/>
+      <c r="AK40" s="2"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="6"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -1832,15 +2522,30 @@
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="2"/>
+      <c r="AE41" s="2"/>
+      <c r="AF41" s="2"/>
+      <c r="AG41" s="2"/>
+      <c r="AH41" s="2"/>
+      <c r="AI41" s="2"/>
+      <c r="AJ41" s="2"/>
+      <c r="AK41" s="2"/>
+      <c r="AL41" s="2"/>
+      <c r="AM41" s="2"/>
+      <c r="AN41" s="2"/>
+      <c r="AO41" s="2"/>
+    </row>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="G42" s="6"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -1860,15 +2565,30 @@
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="2"/>
+      <c r="AE42" s="2"/>
+      <c r="AF42" s="2"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AI42" s="2"/>
+      <c r="AJ42" s="2"/>
+      <c r="AK42" s="2"/>
+      <c r="AL42" s="2"/>
+      <c r="AM42" s="2"/>
+      <c r="AN42" s="2"/>
+      <c r="AO42" s="2"/>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="G43" s="6"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -1888,15 +2608,30 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="2"/>
+      <c r="AE43" s="2"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="2"/>
+      <c r="AI43" s="2"/>
+      <c r="AJ43" s="2"/>
+      <c r="AK43" s="2"/>
+      <c r="AL43" s="2"/>
+      <c r="AM43" s="2"/>
+      <c r="AN43" s="2"/>
+      <c r="AO43" s="2"/>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="G44" s="6"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -1916,15 +2651,30 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="2"/>
+      <c r="AE44" s="2"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="2"/>
+      <c r="AI44" s="2"/>
+      <c r="AJ44" s="2"/>
+      <c r="AK44" s="2"/>
+      <c r="AL44" s="2"/>
+      <c r="AM44" s="2"/>
+      <c r="AN44" s="2"/>
+      <c r="AO44" s="2"/>
+    </row>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="G45" s="6"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -1944,15 +2694,30 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="2"/>
+      <c r="AE45" s="2"/>
+      <c r="AF45" s="2"/>
+      <c r="AG45" s="2"/>
+      <c r="AH45" s="2"/>
+      <c r="AI45" s="2"/>
+      <c r="AJ45" s="2"/>
+      <c r="AK45" s="2"/>
+      <c r="AL45" s="2"/>
+      <c r="AM45" s="2"/>
+      <c r="AN45" s="2"/>
+      <c r="AO45" s="2"/>
+    </row>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -1972,15 +2737,30 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="2"/>
+      <c r="AE46" s="2"/>
+      <c r="AF46" s="2"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="2"/>
+      <c r="AI46" s="2"/>
+      <c r="AJ46" s="2"/>
+      <c r="AK46" s="2"/>
+      <c r="AL46" s="2"/>
+      <c r="AM46" s="2"/>
+      <c r="AN46" s="2"/>
+      <c r="AO46" s="2"/>
+    </row>
+    <row r="47" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="G47" s="6"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2000,15 +2780,30 @@
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA47" s="2"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="2"/>
+      <c r="AE47" s="2"/>
+      <c r="AF47" s="2"/>
+      <c r="AG47" s="2"/>
+      <c r="AH47" s="2"/>
+      <c r="AI47" s="2"/>
+      <c r="AJ47" s="2"/>
+      <c r="AK47" s="2"/>
+      <c r="AL47" s="2"/>
+      <c r="AM47" s="2"/>
+      <c r="AN47" s="2"/>
+      <c r="AO47" s="2"/>
+    </row>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="G48" s="6"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2028,15 +2823,30 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA48" s="2"/>
+      <c r="AB48" s="2"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="2"/>
+      <c r="AE48" s="2"/>
+      <c r="AF48" s="2"/>
+      <c r="AG48" s="2"/>
+      <c r="AH48" s="2"/>
+      <c r="AI48" s="2"/>
+      <c r="AJ48" s="2"/>
+      <c r="AK48" s="2"/>
+      <c r="AL48" s="2"/>
+      <c r="AM48" s="2"/>
+      <c r="AN48" s="2"/>
+      <c r="AO48" s="2"/>
+    </row>
+    <row r="49" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="G49" s="6"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2056,15 +2866,30 @@
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA49" s="2"/>
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="2"/>
+      <c r="AE49" s="2"/>
+      <c r="AF49" s="2"/>
+      <c r="AG49" s="2"/>
+      <c r="AH49" s="2"/>
+      <c r="AI49" s="2"/>
+      <c r="AJ49" s="2"/>
+      <c r="AK49" s="2"/>
+      <c r="AL49" s="2"/>
+      <c r="AM49" s="2"/>
+      <c r="AN49" s="2"/>
+      <c r="AO49" s="2"/>
+    </row>
+    <row r="50" spans="1:41" x14ac:dyDescent="0.35">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="G50" s="6"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2084,86 +2909,33 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+      <c r="AG50" s="2"/>
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="2"/>
+      <c r="AJ50" s="2"/>
+      <c r="AK50" s="2"/>
+      <c r="AL50" s="2"/>
+      <c r="AM50" s="2"/>
+      <c r="AN50" s="2"/>
+      <c r="AO50" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="21">
-    <dataValidation type="list" allowBlank="1" sqref="G2:G50" xr:uid="{EF4CB57A-2FC3-479D-A9B6-7612FD458D32}">
-      <formula1>INDIRECT($G$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="H2:H50" xr:uid="{B12D95CE-5FCD-468C-ACA2-89D6936C7C42}">
-      <formula1>INDIRECT($H$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="I2:I50" xr:uid="{F9C2A7CA-8DB9-4B64-8AE0-B9EE4489DC91}">
-      <formula1>INDIRECT($I$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J50" xr:uid="{61D26EA1-3380-4D06-A0A0-F37CF30341ED}">
-      <formula1>INDIRECT($J$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="K2:K50" xr:uid="{F1C947C6-EC54-4807-B914-247BB2DF8284}">
-      <formula1>INDIRECT($K$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="L2:L50" xr:uid="{74E4FC39-E564-479A-B458-A8D473DFD30C}">
-      <formula1>INDIRECT($L$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="M2:M50" xr:uid="{188A0BF9-E4DF-45E4-A0A2-251DD01923B7}">
-      <formula1>INDIRECT($M$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="N2:N50" xr:uid="{C1DFFF5A-623C-49FE-966D-CD5956E80456}">
-      <formula1>INDIRECT($N$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="O2:O50" xr:uid="{00154250-3FFD-4999-A9A5-FE026631491B}">
-      <formula1>INDIRECT($O$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="P2:P50" xr:uid="{884586FC-8066-4480-8F09-EFC3D72B8CEE}">
-      <formula1>INDIRECT($P$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Q2:Q50" xr:uid="{57855A25-9B3D-4F99-978F-152A56A722C0}">
-      <formula1>INDIRECT($Q$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="R2:R50" xr:uid="{22EBCEFC-59BD-4A40-BC1C-72A639E3DFE6}">
-      <formula1>INDIRECT($R$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="S2:S50" xr:uid="{F5B7978E-80D2-4FF5-A350-BD93DE98382E}">
-      <formula1>INDIRECT($S$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="T2:T50" xr:uid="{2E6514AA-5428-4C2F-A420-1D9D1D47E42E}">
-      <formula1>INDIRECT($T$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="U2:U50" xr:uid="{B10D8F3B-74F5-46AE-8BE6-F94102FFD206}">
-      <formula1>INDIRECT($U$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="V2:V50" xr:uid="{BE7F84A0-4D15-4B75-AB63-933C7DC8E3CA}">
-      <formula1>INDIRECT($V$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="W2:W50" xr:uid="{EA50A479-09B6-411B-8490-197CBC410584}">
-      <formula1>INDIRECT($W$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="X2:X50" xr:uid="{D716BCDA-7540-498D-9153-E2A50E0E6216}">
-      <formula1>INDIRECT($X$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Y2:Y50" xr:uid="{BC5BD409-189A-4BB6-BCF5-79F6C82A536C}">
-      <formula1>INDIRECT($Y$1)</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="Z2:Z50" xr:uid="{960C5FCE-FCF2-4F57-A548-CA470B43C4EB}">
-      <formula1>INDIRECT($Z$1)</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A50" xr:uid="{77034CF6-46F2-42EB-AF6A-5168220E2A74}">
       <formula1>INDIRECT($A$1)</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="G2:AO299" xr:uid="{0263AEB1-382A-4F98-8941-42499E51AB31}">
+      <formula1>INDIRECT(G$1)</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{64339059-9890-4279-A1B1-AEAF06939486}">
-          <x14:formula1>
-            <xm:f>field_list!$A$2:$A$38</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1:Z1</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2171,9 +2943,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9434A0-0E2B-4724-A3F0-82D34619CEAF}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>